<commit_message>
added presentation + screencast in README.md
</commit_message>
<xml_diff>
--- a/Docs/timesheet_brent_de_roeck.xlsx
+++ b/Docs/timesheet_brent_de_roeck.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\School\schooljaar 2018-19\Semester 1\CMS\Eindopdracht\Productiedossier\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\School\schooljaar 2018-19\Semester 1\CMS\Eindopdracht\SleepyRepo\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4124A018-9E3C-4213-9AA3-D4CEB641F0A6}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91FFCBAD-09F8-47E9-8970-515D10A85182}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8424" xr2:uid="{642C154F-05DF-4873-BBA7-2CFE4D2CD992}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="93">
   <si>
     <t>CMSDEV</t>
   </si>
@@ -304,6 +304,12 @@
   </si>
   <si>
     <t>Adding hashtag to posts</t>
+  </si>
+  <si>
+    <t>Screencast maken</t>
+  </si>
+  <si>
+    <t>Presentatie maken</t>
   </si>
 </sst>
 </file>
@@ -680,7 +686,7 @@
   <dimension ref="A1:C105"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A80" workbookViewId="0">
-      <selection activeCell="C96" sqref="C96"/>
+      <selection activeCell="C98" sqref="C98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1732,10 +1738,26 @@
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A96" s="2"/>
+      <c r="A96" s="2">
+        <v>43475</v>
+      </c>
+      <c r="B96" t="s">
+        <v>91</v>
+      </c>
+      <c r="C96">
+        <v>2</v>
+      </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A97" s="2"/>
+      <c r="A97" s="2">
+        <v>43477</v>
+      </c>
+      <c r="B97" t="s">
+        <v>92</v>
+      </c>
+      <c r="C97">
+        <v>1.5</v>
+      </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A98" s="2"/>
@@ -1758,7 +1780,7 @@
     <row r="105" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C105">
         <f>SUM(C3:C104)</f>
-        <v>211.5</v>
+        <v>215</v>
       </c>
     </row>
   </sheetData>

</xml_diff>